<commit_message>
Project sp1 is saved. Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/sp1/Main.xlsx
+++ b/DESIGN/rules/sp1/Main.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A29B8A-3A15-426F-8EEE-ECBCCF0D9655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="4" r:id="rId1"/>
@@ -14,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Stanislav Shor</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -32,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -263,7 +269,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -599,13 +605,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -958,28 +967,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
         <v>21</v>
       </c>
@@ -987,7 +998,7 @@
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1013,7 +1024,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>19</v>
@@ -1025,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
@@ -1039,12 +1050,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="16">
-        <v>0</v>
+        <v>1110</v>
       </c>
       <c r="D8" s="17">
         <v>11</v>
@@ -1053,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -1081,7 +1092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>15</v>
       </c>

</xml_diff>